<commit_message>
emission plots and postprocess
emission default name of CO_2 equivalent has changes to user specified emission name
</commit_message>
<xml_diff>
--- a/examples/Utopia1_operation_multi_node/config.xlsx
+++ b/examples/Utopia1_operation_multi_node/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/negarnamazifard/Documents/GitHub/Hypatia_SESAM/examples/Utopia1_operation_multi_node/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadamintahavori/Documents/GitHub/Hypatia_sesam/examples/Utopia1_operation_multi_node/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341F67AC-96AA-6542-BAA5-402649CB63D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB4D9DE-0F15-0140-B753-0BBBBD27E61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
   <si>
     <t>tech_name</t>
   </si>
@@ -124,9 +124,6 @@
     <t>emission_unit</t>
   </si>
   <si>
-    <t>CO2-equivalent</t>
-  </si>
-  <si>
     <t>Natural Gas Extraction</t>
   </si>
   <si>
@@ -260,6 +257,15 @@
   </si>
   <si>
     <t>#8C564B</t>
+  </si>
+  <si>
+    <t>emission_name</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CO2 emissions</t>
   </si>
 </sst>
 </file>
@@ -664,7 +670,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F12"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -694,19 +700,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -714,19 +720,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -734,19 +740,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
         <v>44</v>
       </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -754,19 +760,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -774,19 +780,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
         <v>48</v>
       </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
-      </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -794,19 +800,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -814,19 +820,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
         <v>52</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -834,19 +840,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
         <v>55</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -854,19 +860,19 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>59</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>60</v>
       </c>
-      <c r="E10" t="s">
-        <v>61</v>
-      </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -874,19 +880,19 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
         <v>62</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>63</v>
       </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -894,19 +900,19 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" t="s">
-        <v>66</v>
-      </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -919,7 +925,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -946,16 +952,16 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -963,16 +969,16 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -980,16 +986,16 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
         <v>70</v>
       </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -997,16 +1003,16 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
         <v>72</v>
       </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1020,10 +1026,10 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1035,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1057,10 +1063,10 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
         <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1068,10 +1074,10 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
         <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1081,25 +1087,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>